<commit_message>
Status and type graphs.
</commit_message>
<xml_diff>
--- a/Output/OSC/DOE/DOE_Assistance.xlsx
+++ b/Output/OSC/DOE/DOE_Assistance.xlsx
@@ -7,12 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="Crit" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Status" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Type" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">program</t>
   </si>
@@ -69,15 +71,58 @@
   </si>
   <si>
     <t xml:space="preserve">Grand Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Commitment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISCONTINUED PROJECTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discontinued Projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INACTIVE CONDITIONAL COMMITMENTS�</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECTS THAT CLOSED ON LOANS BUT RECEIVED NO DISBURSEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repaid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direct Loan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loan Guarantee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loan TypeLoan Guarantee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Loan Guarantee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
+  <numFmts count="3">
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="171" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -113,10 +158,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,29 +519,29 @@
       <c r="M2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="n">
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="n">
         <v>21730000000</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="n">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="n">
         <v>2802000000</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="n">
+      <c r="S2" s="1"/>
+      <c r="T2" s="1" t="n">
         <v>375000000</v>
       </c>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -504,47 +550,47 @@
       <c r="M3" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="2" t="n">
+      <c r="N3" s="1" t="n">
         <v>1040000000</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="O3" s="1" t="n">
         <v>11500000000</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2" t="n">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="n">
         <v>1162000000</v>
       </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2" t="n">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="n">
         <v>504000000</v>
       </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2" t="n">
+      <c r="T3" s="1"/>
+      <c r="U3" s="1" t="n">
         <v>5883000000</v>
       </c>
-      <c r="V3" s="2" t="n">
+      <c r="V3" s="1" t="n">
         <v>545000000</v>
       </c>
-      <c r="W3" s="2" t="n">
+      <c r="W3" s="1" t="n">
         <v>1688000000</v>
       </c>
-      <c r="X3" s="2" t="n">
+      <c r="X3" s="1" t="n">
         <v>6095600000</v>
       </c>
-      <c r="Y3" s="2" t="n">
+      <c r="Y3" s="1" t="n">
         <v>1232978000</v>
       </c>
-      <c r="Z3" s="2" t="n">
+      <c r="Z3" s="1" t="n">
         <v>458000000</v>
       </c>
-      <c r="AA3" s="2" t="n">
+      <c r="AA3" s="1" t="n">
         <v>343000000</v>
       </c>
-      <c r="AB3" s="2" t="n">
+      <c r="AB3" s="1" t="n">
         <v>3000000000</v>
       </c>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -553,53 +599,53 @@
       <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="2" t="str">
+      <c r="N4" s="1" t="str">
         <f>Sum(N2:N3)</f>
       </c>
-      <c r="O4" s="2" t="str">
+      <c r="O4" s="1" t="str">
         <f>Sum(O2:O3)</f>
       </c>
-      <c r="P4" s="2" t="str">
+      <c r="P4" s="1" t="str">
         <f>Sum(P2:P3)</f>
       </c>
-      <c r="Q4" s="2" t="str">
+      <c r="Q4" s="1" t="str">
         <f>Sum(Q2:Q3)</f>
       </c>
-      <c r="R4" s="2" t="str">
+      <c r="R4" s="1" t="str">
         <f>Sum(R2:R3)</f>
       </c>
-      <c r="S4" s="2" t="str">
+      <c r="S4" s="1" t="str">
         <f>Sum(S2:S3)</f>
       </c>
-      <c r="T4" s="2" t="str">
+      <c r="T4" s="1" t="str">
         <f>Sum(T2:T3)</f>
       </c>
-      <c r="U4" s="2" t="str">
+      <c r="U4" s="1" t="str">
         <f>Sum(U2:U3)</f>
       </c>
-      <c r="V4" s="2" t="str">
+      <c r="V4" s="1" t="str">
         <f>Sum(V2:V3)</f>
       </c>
-      <c r="W4" s="2" t="str">
+      <c r="W4" s="1" t="str">
         <f>Sum(W2:W3)</f>
       </c>
-      <c r="X4" s="2" t="str">
+      <c r="X4" s="1" t="str">
         <f>Sum(X2:X3)</f>
       </c>
-      <c r="Y4" s="2" t="str">
+      <c r="Y4" s="1" t="str">
         <f>Sum(Y2:Y3)</f>
       </c>
-      <c r="Z4" s="2" t="str">
+      <c r="Z4" s="1" t="str">
         <f>Sum(Z2:Z3)</f>
       </c>
-      <c r="AA4" s="2" t="str">
+      <c r="AA4" s="1" t="str">
         <f>Sum(AA2:AA3)</f>
       </c>
-      <c r="AB4" s="2" t="str">
+      <c r="AB4" s="1" t="str">
         <f>Sum(AB2:AB3)</f>
       </c>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -655,25 +701,25 @@
       <c r="M8" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2" t="n">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1" t="n">
         <v>13431599000.2096</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2" t="n">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1" t="n">
         <v>102000000</v>
       </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -682,43 +728,279 @@
       <c r="M9" t="s">
         <v>17</v>
       </c>
+      <c r="N9" s="1" t="n">
+        <v>13951782276.4929</v>
+      </c>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1" t="n">
+        <v>1490128919.88848</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1" t="n">
+        <v>504000000</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <v>7544258550.51972</v>
+      </c>
+      <c r="T9" s="1" t="n">
+        <v>701431468.663747</v>
+      </c>
+      <c r="U9" s="1" t="n">
+        <v>2167686165.28201</v>
+      </c>
+      <c r="V9" s="1" t="n">
+        <v>7758416493.39526</v>
+      </c>
+      <c r="W9" s="1" t="n">
+        <v>1601064253.00539</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <v>78054300.9467365</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <v>439857331.77431</v>
+      </c>
+      <c r="Z9" s="1" t="n">
+        <v>2861395138.30596</v>
+      </c>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <f>M10</f>
+      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <f>M1</f>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <f>M2</f>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>2602000000</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>13652000000</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>579000000</v>
+      </c>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2" t="n">
+        <v>259000000</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2" t="n">
+        <v>7815000000</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <f>M3</f>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>26096000000</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>1438000000</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>1270000000</v>
+      </c>
+      <c r="Q3" s="2" t="n">
+        <v>459000000</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>2774978000</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>1368000000</v>
+      </c>
+      <c r="U3" s="2" t="n">
+        <v>45600000</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <f>M4</f>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="2" t="str">
+        <f>Sum(N2:N3)</f>
+      </c>
+      <c r="O4" s="2" t="str">
+        <f>Sum(O2:O3)</f>
+      </c>
+      <c r="P4" s="2" t="str">
+        <f>Sum(P2:P3)</f>
+      </c>
+      <c r="Q4" s="2" t="str">
+        <f>Sum(Q2:Q3)</f>
+      </c>
+      <c r="R4" s="2" t="str">
+        <f>Sum(R2:R3)</f>
+      </c>
+      <c r="S4" s="2" t="str">
+        <f>Sum(S2:S3)</f>
+      </c>
+      <c r="T4" s="2" t="str">
+        <f>Sum(T2:T3)</f>
+      </c>
+      <c r="U4" s="2" t="str">
+        <f>Sum(U2:U3)</f>
+      </c>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <f>M7</f>
+      </c>
+      <c r="M7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <f>M8</f>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="2" t="n">
+        <v>2486495948.5883</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>756171606.383545</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2" t="n">
+        <v>10290931445.2378</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <f>M9</f>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
       <c r="N9" s="2" t="n">
-        <v>13951782276.4929</v>
-      </c>
-      <c r="O9" s="2"/>
+        <v>31541368446.9873</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>1649651959.87192</v>
+      </c>
       <c r="P9" s="2" t="n">
-        <v>1490128919.88848</v>
-      </c>
-      <c r="Q9" s="2"/>
+        <v>588613747.184863</v>
+      </c>
+      <c r="Q9" s="2" t="n">
+        <v>3558584311.40644</v>
+      </c>
       <c r="R9" s="2" t="n">
-        <v>504000000</v>
-      </c>
-      <c r="S9" s="2" t="n">
-        <v>7544258550.51972</v>
-      </c>
-      <c r="T9" s="2" t="n">
-        <v>701431468.663747</v>
-      </c>
-      <c r="U9" s="2" t="n">
-        <v>2167686165.28201</v>
-      </c>
-      <c r="V9" s="2" t="n">
-        <v>7758416493.39526</v>
-      </c>
-      <c r="W9" s="2" t="n">
-        <v>1601064253.00539</v>
-      </c>
-      <c r="X9" s="2" t="n">
-        <v>78054300.9467365</v>
-      </c>
-      <c r="Y9" s="2" t="n">
-        <v>439857331.77431</v>
-      </c>
-      <c r="Z9" s="2" t="n">
-        <v>2861395138.30596</v>
-      </c>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
+        <v>1759856432.82395</v>
+      </c>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -731,14 +1013,207 @@
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane ySplit="1" xSplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <f>M1</f>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <f>M2</f>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>9200000000</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <f>M3</f>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>14869000000</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3" t="n">
+        <v>838000000</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <f>M4</f>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="n">
+        <v>21290000000</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>343000000</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>7269000000</v>
+      </c>
+      <c r="R4" s="3" t="n">
+        <v>4549578000</v>
+      </c>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <f>M5</f>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="3" t="str">
+        <f>Sum(N2:N4)</f>
+      </c>
+      <c r="O5" s="3" t="str">
+        <f>Sum(O2:O4)</f>
+      </c>
+      <c r="P5" s="3" t="str">
+        <f>Sum(P2:P4)</f>
+      </c>
+      <c r="Q5" s="3" t="str">
+        <f>Sum(Q2:Q4)</f>
+      </c>
+      <c r="R5" s="3" t="str">
+        <f>Sum(R2:R4)</f>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <f>M8</f>
+      </c>
+      <c r="M8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <f>M9</f>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="3" t="n">
+        <v>12777427393.8261</v>
+      </c>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3" t="n">
+        <v>756171606.383545</v>
+      </c>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <f>M10</f>
+      </c>
+      <c r="M10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3" t="n">
+        <v>24522947053.2319</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>439857331.77431</v>
+      </c>
+      <c r="Q10" s="3" t="n">
+        <v>8338420494.80507</v>
+      </c>
+      <c r="R10" s="3" t="n">
+        <v>5796850018.46323</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <f>M11</f>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>